<commit_message>
chore: 更新 AScan 模板文件
- 修改了 excel_templates/AScan/T_模板.xlsx 文件
</commit_message>
<xml_diff>
--- a/excel_templates/AScan/T_仪器性能.xlsx
+++ b/excel_templates/AScan/T_仪器性能.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\UnionOffline\UnionOffline\excel_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\UnionOffline\UnionOffline\excel_templates\AScan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610C4D21-9955-4C79-AA12-84070255BB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4466A5B7-4C37-4824-A756-AD998BFFDC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -379,21 +379,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -703,7 +700,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -726,7 +723,7 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -734,7 +731,7 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -742,7 +739,7 @@
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -750,7 +747,7 @@
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -758,7 +755,7 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -766,15 +763,15 @@
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="35.1" customHeight="1">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>